<commit_message>
reporter: Use the term "issue" instead of "error"
Esp. in all user-facing code, use the term "issue" instead of the legacy
"error" term. Also rename most variables / functions in the reporter,
but do not touch any code from the "model" to keep the diff reasonably
small for review. More renaming throughout the code base will follow
later.

Signed-off-by: Sebastian Schuberth <sebastian.schuberth@here.com>
</commit_message>
<xml_diff>
--- a/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
+++ b/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
@@ -67,10 +67,10 @@
     <t>Detected Licenses</t>
   </si>
   <si>
-    <t>Analyzer Errors</t>
-  </si>
-  <si>
-    <t>Scan Errors</t>
+    <t>Analyzer Issues</t>
+  </si>
+  <si>
+    <t>Scan Issues</t>
   </si>
   <si>
     <r>
@@ -444,7 +444,7 @@
     <col min="2" max="2" width="41.45703125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.8828125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="17.4296875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="14.9765625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.00390625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="254.4453125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -650,7 +650,7 @@
     <col min="2" max="2" width="11.81640625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.8828125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="17.4296875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="14.9765625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.00390625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="254.4453125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
OrtIssue: Say "Unknown time" instead of "n/a"
Otherwise it is unclear what "n/a" refers to in the message.

Signed-off-by: Sebastian Schuberth <sebastian.schuberth@here.com>
</commit_message>
<xml_diff>
--- a/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
+++ b/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
@@ -98,7 +98,7 @@
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Gradle:com.here.ort.gradle.example:lib:1.0.0
-  n/a: FileCounter - DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
+  Unknown time: FileCounter - DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
 Caused by: DownloadException: No VCS URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'. Please make sure the release POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#example_customizing_the_pom_file
 </t>
     </r>
@@ -222,7 +222,7 @@
         <sz val="11.0"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>n/a: FileCounter - DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
+      <t>Unknown time: FileCounter - DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
 Caused by: DownloadException: No VCS URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'. Please make sure the release POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#example_customizing_the_pom_file</t>
     </r>
   </si>

</xml_diff>

<commit_message>
OrtIssue: Add the severity to the string representation
Otherwise it is a bit unclear what e.g. the different row colors in the
static HTML report stand for.

Signed-off-by: Sebastian Schuberth <sebastian.schuberth@here.com>
</commit_message>
<xml_diff>
--- a/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
+++ b/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
@@ -98,7 +98,7 @@
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Gradle:com.here.ort.gradle.example:lib:1.0.0
-  Unknown time: FileCounter - DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
+  Unknown time [ERROR]: FileCounter - DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
 Caused by: DownloadException: No VCS URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'. Please make sure the release POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#example_customizing_the_pom_file
 </t>
     </r>
@@ -222,7 +222,7 @@
         <sz val="11.0"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>Unknown time: FileCounter - DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
+      <t>Unknown time [ERROR]: FileCounter - DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
 Caused by: DownloadException: No VCS URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'. Please make sure the release POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#example_customizing_the_pom_file</t>
     </r>
   </si>

</xml_diff>

<commit_message>
LicenseInfoResolver: Add original license source to ResolvedLicenseInfo
This is required to apply choices to the expression at a later point in
time.

Signed-off-by: Marcel Bochtler <marcel.bochtler@bosch.io>
</commit_message>
<xml_diff>
--- a/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
+++ b/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\oss-review-toolkit\reporter\src\funTest\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sse1be\Development\GitHub\oss-review-toolkit\ort\reporter\src\funTest\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E48ABD-96E1-4177-8D38-DE1E74EEF156}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5F3D68-2701-4389-8F27-EFE65A4E6A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="2955" windowWidth="26190" windowHeight="15015" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -228,15 +228,6 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>ResolvedLicense(license=EPL-1.0, sources=[DECLARED], originalDeclaredLicenses=[Eclipse Public License 1.0], locations=[])</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
       <t xml:space="preserve">compile
 </t>
     </r>
@@ -247,24 +238,6 @@
       </rPr>
       <t xml:space="preserve">testCompile
 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>ResolvedLicense(license=Apache-2.0, sources=[DECLARED], originalDeclaredLicenses=[Apache License, Version 2.0], locations=[])</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>ResolvedLicense(license=BSD-3-Clause, sources=[DECLARED], originalDeclaredLicenses=[New BSD License], locations=[])</t>
     </r>
   </si>
   <si>
@@ -279,12 +252,21 @@
 Suppressed: DownloadException: No VCS URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'. Please make sure the published POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#sec:modifying_the_generated_pom
 Suppressed: DownloadException: No source artifact URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.</t>
   </si>
+  <si>
+    <t>ResolvedLicense(license=EPL-1.0, originalDeclaredLicenses=[Eclipse Public License 1.0], originalExpressions={DECLARED=[EPL-1.0]}, locations=[])</t>
+  </si>
+  <si>
+    <t>ResolvedLicense(license=Apache-2.0, originalDeclaredLicenses=[Apache License, Version 2.0], originalExpressions={DECLARED=[Apache-2.0]}, locations=[])</t>
+  </si>
+  <si>
+    <t>ResolvedLicense(license=BSD-3-Clause, originalDeclaredLicenses=[New BSD License], originalExpressions={DECLARED=[BSD-3-Clause]}, locations=[])</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -347,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -371,9 +353,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -389,7 +374,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -694,7 +679,7 @@
       <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
@@ -703,7 +688,7 @@
     <col min="6" max="6" width="229.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -715,7 +700,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -727,12 +712,12 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -744,7 +729,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -756,7 +741,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -768,7 +753,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -780,7 +765,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -800,7 +785,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1">
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -817,10 +802,10 @@
         <v>8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -840,7 +825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="75" customHeight="1">
+    <row r="13" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -860,7 +845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="75" customHeight="1">
+    <row r="14" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -880,7 +865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="45" customHeight="1">
+    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -919,13 +904,13 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -935,7 +920,7 @@
     <col min="6" max="6" width="229.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -947,7 +932,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -959,12 +944,12 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -976,7 +961,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -988,7 +973,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1000,7 +985,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1012,7 +997,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1032,7 +1017,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1047,18 +1032,18 @@
         <v>8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>32</v>
+      <c r="C12" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -1070,15 +1055,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1">
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -1090,15 +1075,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1">
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -1110,15 +1095,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>35</v>
+      <c r="C15" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>

</xml_diff>